<commit_message>
finished putawaynote print and fixed bugs
</commit_message>
<xml_diff>
--- a/UI/bin/Debug/Excel/PutAwayNote.xlsx
+++ b/UI/bin/Debug/Excel/PutAwayNote.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Visual Studio 2017\Projects\WMSClient\UI\bin\Debug\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1B4E059F-B8C3-4A88-AAFA-BDE8FEB2C354}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29B2BC46-ED84-49D6-A8D5-12685FDA2326}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20412" windowHeight="10572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>#SET TABLE COLUMNS 11</t>
   </si>
@@ -28,21 +28,6 @@
     <t>上架作业单</t>
   </si>
   <si>
-    <t>时间:@ticket.CreateTime.toLocaleDateString();</t>
-  </si>
-  <si>
-    <t>仓库:@ticket.WarehouseName</t>
-  </si>
-  <si>
-    <t>项目:@ticket.ProjectName</t>
-  </si>
-  <si>
-    <t>作业组:@ticket.JobGroupName</t>
-  </si>
-  <si>
-    <t>内向交货单:@ticket.InwardDeliverTicketNo</t>
-  </si>
-  <si>
     <t>零件号</t>
   </si>
   <si>
@@ -68,46 +53,50 @@
   </si>
   <si>
     <t>#WRITE var ticket=putAwayTicket;var item=putAwayTicketItems;""</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE item[i].materialName</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE item[i].materialNo</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE item[i].supplierName</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>#WRITE item[i].inventoryDate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE ticket.no</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE item[i].targetStorageLocationName</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE item[i].scheduledAmount</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>#WRITE item[i].realAmount</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间:@ticket.createTime;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓库:@ticket.warehouseName</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,19 +126,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="黑体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="黑体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -164,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -187,6 +163,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -200,9 +202,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -220,9 +219,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,6 +230,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -528,219 +530,202 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="K1" s="7"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="K4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="4" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="H2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>